<commit_message>
OVW sheet updated with added variation in product listing.
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_product_listing.xlsx
+++ b/docs/OVW Sheets/OVWDemo_product_listing.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samaddel\Desktop\QA\7 dec\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755" firstSheet="35" activeTab="47"/>
   </bookViews>
   <sheets>
     <sheet name="de_de" sheetId="1" r:id="rId1"/>
@@ -71,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="425">
   <si>
     <t>http://www.cisco.com/web/DE/products/telepresence/products.html</t>
   </si>
@@ -1343,6 +1338,9 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/BE/fr/solutions/borderless/prodportfolio.html</t>
+  </si>
+  <si>
+    <t>product-listing-var7</t>
   </si>
 </sst>
 </file>
@@ -1502,7 +1500,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1537,7 +1535,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1714,7 +1712,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1724,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1802,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -1908,7 +1906,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1980,7 +1978,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2078,7 +2076,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2140,7 +2138,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2227,7 +2225,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,7 +2295,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2394,7 +2392,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,7 +2464,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2564,7 +2562,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2636,7 +2634,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2734,7 +2732,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2804,7 +2802,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -2901,7 +2899,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2965,7 +2963,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -3052,7 +3050,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3124,7 +3122,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -3222,7 +3220,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3296,7 +3294,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -3394,7 +3392,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3466,7 +3464,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -3564,7 +3562,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3637,7 +3635,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -3734,7 +3732,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3806,7 +3804,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -3904,7 +3902,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3966,7 +3964,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -4202,7 +4200,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4274,7 +4272,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -4372,7 +4370,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4444,7 +4442,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -4542,7 +4540,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4604,7 +4602,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -4691,7 +4689,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4771,7 +4769,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -4869,7 +4867,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4948,7 +4946,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -5051,7 +5049,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5130,7 +5128,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -5234,7 +5232,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5314,7 +5312,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -5418,7 +5416,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5490,7 +5488,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -5588,7 +5586,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5660,7 +5658,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -5758,7 +5756,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5830,7 +5828,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -5928,7 +5926,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6002,7 +6000,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -6100,7 +6098,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6175,7 +6173,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -6273,7 +6271,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6348,7 +6346,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -6446,7 +6444,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6521,7 +6519,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -6785,7 +6783,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6860,7 +6858,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -6958,7 +6956,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7033,7 +7031,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -7131,7 +7129,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7205,7 +7203,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -7303,7 +7301,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7375,7 +7373,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -7473,7 +7471,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7548,7 +7546,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -7646,7 +7644,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7721,7 +7719,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -7819,7 +7817,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7894,7 +7892,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -7991,7 +7989,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8066,7 +8064,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8164,7 +8162,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8239,7 +8237,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8330,7 +8328,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8404,7 +8402,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8502,7 +8500,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8576,7 +8574,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8674,7 +8672,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8748,7 +8746,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -8845,8 +8843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8920,7 +8918,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -9018,7 +9016,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9090,7 +9088,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -9188,7 +9186,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9260,7 +9258,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -9358,7 +9356,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9430,7 +9428,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -9528,7 +9526,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9600,7 +9598,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -9697,7 +9695,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9767,7 +9765,7 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>424</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
OVWDemo sheet corrected for Product Listing RU Locale.
</commit_message>
<xml_diff>
--- a/docs/OVW Sheets/OVWDemo_product_listing.xlsx
+++ b/docs/OVW Sheets/OVWDemo_product_listing.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="7755" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="de_de" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="434">
   <si>
     <t>http://www.cisco.com/web/DE/products/telepresence/products.html</t>
   </si>
@@ -1338,6 +1338,36 @@
   </si>
   <si>
     <t>product-listing-var7</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/telepresence/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/webex/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/collaboration/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/voice/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/sp/product-listing.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/uc/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/products/storage/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/collaboration/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/datacenter/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/RU/solutions/borderless/prodportfolio.html</t>
   </si>
 </sst>
 </file>
@@ -1428,7 +1458,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1436,6 +1466,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1709,7 +1740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1719,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -6636,8 +6667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6646,8 +6677,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>34</v>
+      <c r="A1" s="7" t="s">
+        <v>424</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -6661,7 +6692,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>35</v>
+        <v>425</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -6675,7 +6706,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>36</v>
+        <v>426</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -6689,7 +6720,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>37</v>
+        <v>427</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -6703,7 +6734,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>428</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -6717,7 +6748,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>429</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -6730,8 +6761,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>40</v>
+      <c r="A7" s="1" t="s">
+        <v>430</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -6744,8 +6775,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>41</v>
+      <c r="A8" s="2" t="s">
+        <v>431</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
@@ -6758,8 +6789,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>42</v>
+      <c r="A9" s="2" t="s">
+        <v>432</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -6772,8 +6803,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>43</v>
+      <c r="A10" s="2" t="s">
+        <v>433</v>
       </c>
       <c r="B10" t="s">
         <v>24</v>
@@ -6788,17 +6819,17 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="A2" r:id="rId2"/>
-    <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="A5" r:id="rId5"/>
-    <hyperlink ref="A6" r:id="rId6" display="http://www.cisco.com/cisco/web/UK/products/unified_computing/services.html"/>
-    <hyperlink ref="A7" r:id="rId7"/>
-    <hyperlink ref="A8" r:id="rId8"/>
-    <hyperlink ref="A9" r:id="rId9"/>
-    <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+    <hyperlink ref="A7" r:id="rId6"/>
+    <hyperlink ref="A8" r:id="rId7"/>
+    <hyperlink ref="A9" r:id="rId8"/>
+    <hyperlink ref="A10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>